<commit_message>
add in mendocino county data
</commit_message>
<xml_diff>
--- a/data/raw/Mackerricher_HASE_Counts_Pre2018.xlsx
+++ b/data/raw/Mackerricher_HASE_Counts_Pre2018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GERRATY/Coyote_HASE_Predation/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336D50D1-1404-B34A-8F0E-A9BB2BD1E07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A820779F-EFE3-BA41-A161-55BD783F9D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16420" xr2:uid="{73228081-2665-3149-9C4A-CBB35F3C1C96}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{73228081-2665-3149-9C4A-CBB35F3C1C96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,15 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
   <si>
     <t>Time</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>R</t>
@@ -55,9 +52,6 @@
   </si>
   <si>
     <t>Adult</t>
-  </si>
-  <si>
-    <t>Pups</t>
   </si>
   <si>
     <t>S</t>
@@ -112,6 +106,9 @@
   </si>
   <si>
     <t>Swell</t>
+  </si>
+  <si>
+    <t>Pup</t>
   </si>
 </sst>
 </file>
@@ -483,7 +480,7 @@
   <dimension ref="A1:I137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -496,25 +493,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -528,7 +525,7 @@
         <v>1.5</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>73</v>
@@ -536,15 +533,7 @@
       <c r="F2">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -557,7 +546,7 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>34</v>
@@ -566,13 +555,11 @@
         <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="H3" s="4"/>
       <c r="I3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -586,7 +573,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>44</v>
@@ -595,13 +582,10 @@
         <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -615,23 +599,13 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>38</v>
       </c>
-      <c r="F5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" t="s">
-        <v>2</v>
-      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -644,7 +618,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>35</v>
@@ -652,14 +626,10 @@
       <c r="F6">
         <v>20</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
       <c r="I6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -673,7 +643,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <v>36</v>
@@ -682,12 +652,9 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -702,23 +669,13 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <v>70</v>
       </c>
-      <c r="F8" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" t="s">
-        <v>2</v>
-      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -731,7 +688,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <v>60</v>
@@ -739,15 +696,8 @@
       <c r="F9">
         <v>40</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" t="s">
-        <v>2</v>
-      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -760,7 +710,7 @@
         <v>1.5</v>
       </c>
       <c r="D10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <v>56</v>
@@ -769,13 +719,13 @@
         <v>4</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -789,7 +739,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11">
         <v>46</v>
@@ -798,13 +748,13 @@
         <v>5</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -818,7 +768,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <v>58</v>
@@ -827,13 +777,13 @@
         <v>6</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -847,7 +797,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13">
         <v>54</v>
@@ -856,13 +806,13 @@
         <v>7</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" t="s">
         <v>11</v>
-      </c>
-      <c r="I13" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -876,7 +826,7 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14">
         <v>67</v>
@@ -885,13 +835,13 @@
         <v>9</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -905,22 +855,16 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" t="s">
         <v>2</v>
       </c>
       <c r="F15">
         <v>7</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -934,7 +878,7 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16">
         <v>85</v>
@@ -943,13 +887,13 @@
         <v>29</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" t="s">
         <v>11</v>
-      </c>
-      <c r="I16" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -963,36 +907,20 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" t="s">
         <v>2</v>
       </c>
       <c r="F17">
         <v>27</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I17" t="s">
-        <v>2</v>
-      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>40663</v>
       </c>
-      <c r="B18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>2</v>
-      </c>
       <c r="D18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18">
         <v>88</v>
@@ -1000,15 +928,8 @@
       <c r="F18">
         <v>24</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I18" t="s">
-        <v>2</v>
-      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -1021,7 +942,7 @@
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19">
         <v>81</v>
@@ -1029,28 +950,18 @@
       <c r="F19">
         <v>35</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I19" t="s">
-        <v>2</v>
-      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>40664</v>
       </c>
-      <c r="B20" t="s">
-        <v>2</v>
-      </c>
       <c r="C20">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20">
         <v>30</v>
@@ -1058,15 +969,8 @@
       <c r="F20">
         <v>21</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I20" t="s">
-        <v>2</v>
-      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1079,7 +983,7 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E21">
         <v>92</v>
@@ -1088,13 +992,10 @@
         <v>26</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1108,7 +1009,7 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E22">
         <v>58</v>
@@ -1117,13 +1018,10 @@
         <v>22</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I22" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1137,7 +1035,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E23">
         <v>61</v>
@@ -1145,15 +1043,8 @@
       <c r="F23">
         <v>27</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I23" t="s">
-        <v>2</v>
-      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
@@ -1166,7 +1057,7 @@
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E24">
         <v>60</v>
@@ -1174,15 +1065,8 @@
       <c r="F24">
         <v>2</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I24" t="s">
-        <v>2</v>
-      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -1195,23 +1079,15 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E25">
         <v>42</v>
       </c>
-      <c r="F25" t="s">
-        <v>2</v>
-      </c>
       <c r="G25" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I25" t="s">
-        <v>2</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
@@ -1224,23 +1100,13 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E26">
         <v>41</v>
       </c>
-      <c r="F26" t="s">
-        <v>2</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I26" t="s">
-        <v>2</v>
-      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -1253,22 +1119,19 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E27">
         <v>28</v>
       </c>
-      <c r="F27" t="s">
-        <v>2</v>
-      </c>
       <c r="G27" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1282,22 +1145,16 @@
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E28">
         <v>35</v>
       </c>
-      <c r="F28" t="s">
-        <v>2</v>
-      </c>
       <c r="G28" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -1311,7 +1168,7 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29">
         <v>43</v>
@@ -1320,13 +1177,10 @@
         <v>1</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I29" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -1340,7 +1194,7 @@
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E30">
         <v>64</v>
@@ -1349,13 +1203,13 @@
         <v>1</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I30" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -1369,23 +1223,15 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E31">
         <v>10</v>
       </c>
-      <c r="F31" t="s">
-        <v>2</v>
-      </c>
       <c r="G31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I31" t="s">
-        <v>2</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
@@ -1398,7 +1244,7 @@
         <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E32">
         <v>29</v>
@@ -1407,14 +1253,9 @@
         <v>3</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I32" t="s">
-        <v>2</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
@@ -1427,23 +1268,15 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>3</v>
-      </c>
-      <c r="E33" t="s">
         <v>2</v>
       </c>
       <c r="F33">
         <v>13</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I33" t="s">
-        <v>2</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
@@ -1456,7 +1289,7 @@
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E34">
         <v>78</v>
@@ -1464,15 +1297,8 @@
       <c r="F34">
         <v>11</v>
       </c>
-      <c r="G34" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I34" t="s">
-        <v>2</v>
-      </c>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
@@ -1485,7 +1311,7 @@
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E35">
         <v>20</v>
@@ -1494,13 +1320,10 @@
         <v>6</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I35" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -1514,23 +1337,13 @@
         <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>3</v>
-      </c>
-      <c r="E36" t="s">
         <v>2</v>
       </c>
       <c r="F36">
         <v>40</v>
       </c>
-      <c r="G36" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I36" t="s">
-        <v>2</v>
-      </c>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
@@ -1543,23 +1356,14 @@
         <v>2.5</v>
       </c>
       <c r="D37" t="s">
-        <v>3</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E37" s="4"/>
       <c r="F37">
         <v>41</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I37" t="s">
-        <v>2</v>
-      </c>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
@@ -1572,7 +1376,7 @@
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E38">
         <v>71</v>
@@ -1581,13 +1385,13 @@
         <v>40</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -1601,23 +1405,16 @@
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E39">
         <v>65</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="F39" s="4"/>
       <c r="G39" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I39" t="s">
-        <v>2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="H39" s="4"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
@@ -1630,22 +1427,20 @@
         <v>2.75</v>
       </c>
       <c r="D40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E40">
         <v>59</v>
       </c>
-      <c r="F40" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="F40" s="4"/>
       <c r="G40" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I40" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -1659,7 +1454,7 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E41">
         <v>66</v>
@@ -1668,13 +1463,10 @@
         <v>10</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I41" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -1688,7 +1480,7 @@
         <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E42">
         <v>123</v>
@@ -1696,14 +1488,10 @@
       <c r="F42">
         <v>25</v>
       </c>
-      <c r="G42" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
       <c r="I42" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -1717,7 +1505,7 @@
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E43">
         <v>53</v>
@@ -1726,13 +1514,10 @@
         <v>20</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I43" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -1746,7 +1531,7 @@
         <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E44">
         <v>73</v>
@@ -1755,13 +1540,10 @@
         <v>23</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I44" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -1775,7 +1557,7 @@
         <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E45">
         <v>87</v>
@@ -1784,13 +1566,10 @@
         <v>49</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I45" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -1804,7 +1583,7 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E46">
         <v>110</v>
@@ -1813,14 +1592,9 @@
         <v>35</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I46" t="s">
-        <v>2</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="H46" s="4"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
@@ -1833,7 +1607,7 @@
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E47">
         <v>76</v>
@@ -1842,13 +1616,10 @@
         <v>33</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I47" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -1862,7 +1633,7 @@
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E48">
         <v>43</v>
@@ -1871,14 +1642,9 @@
         <v>7</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I48" t="s">
-        <v>2</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H48" s="4"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
@@ -1891,22 +1657,20 @@
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E49">
         <v>35</v>
       </c>
-      <c r="F49" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="F49" s="4"/>
       <c r="G49" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H49" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I49" t="s">
         <v>11</v>
-      </c>
-      <c r="I49" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -1920,23 +1684,14 @@
         <v>1.5</v>
       </c>
       <c r="D50" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E50">
         <v>69</v>
       </c>
-      <c r="F50" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I50" t="s">
-        <v>2</v>
-      </c>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
@@ -1949,23 +1704,14 @@
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E51">
         <v>31</v>
       </c>
-      <c r="F51" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I51" t="s">
-        <v>2</v>
-      </c>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
@@ -1978,23 +1724,16 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E52">
         <v>65</v>
       </c>
-      <c r="F52" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="F52" s="4"/>
       <c r="G52" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I52" t="s">
-        <v>2</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H52" s="4"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
@@ -2007,23 +1746,14 @@
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E53">
         <v>50</v>
       </c>
-      <c r="F53" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H53" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I53" t="s">
-        <v>2</v>
-      </c>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
@@ -2036,23 +1766,14 @@
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E54">
         <v>35</v>
       </c>
-      <c r="F54" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H54" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I54" t="s">
-        <v>2</v>
-      </c>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
@@ -2065,23 +1786,14 @@
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E55">
         <v>85</v>
       </c>
-      <c r="F55" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I55" t="s">
-        <v>2</v>
-      </c>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
@@ -2094,23 +1806,14 @@
         <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E56">
         <v>65</v>
       </c>
-      <c r="F56" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I56" t="s">
-        <v>2</v>
-      </c>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
@@ -2123,23 +1826,14 @@
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E57">
         <v>38</v>
       </c>
-      <c r="F57" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I57" t="s">
-        <v>2</v>
-      </c>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
@@ -2152,23 +1846,14 @@
         <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E58">
         <v>39</v>
       </c>
-      <c r="F58" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I58" t="s">
-        <v>2</v>
-      </c>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
@@ -2181,7 +1866,7 @@
         <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E59">
         <v>80</v>
@@ -2189,15 +1874,8 @@
       <c r="F59">
         <v>4</v>
       </c>
-      <c r="G59" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I59" t="s">
-        <v>2</v>
-      </c>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
@@ -2210,7 +1888,7 @@
         <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E60">
         <v>65</v>
@@ -2218,15 +1896,8 @@
       <c r="F60">
         <v>4</v>
       </c>
-      <c r="G60" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H60" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I60" t="s">
-        <v>2</v>
-      </c>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
@@ -2239,7 +1910,7 @@
         <v>2.5</v>
       </c>
       <c r="D61" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E61">
         <v>50</v>
@@ -2248,14 +1919,9 @@
         <v>15</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H61" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I61" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H61" s="4"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
@@ -2268,7 +1934,7 @@
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E62">
         <v>91</v>
@@ -2277,14 +1943,9 @@
         <v>17</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H62" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I62" t="s">
-        <v>2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="H62" s="4"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
@@ -2297,7 +1958,7 @@
         <v>3</v>
       </c>
       <c r="D63" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E63">
         <v>121</v>
@@ -2306,13 +1967,10 @@
         <v>24</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I63" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
@@ -2326,7 +1984,7 @@
         <v>1.5</v>
       </c>
       <c r="D64" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E64">
         <v>82</v>
@@ -2334,15 +1992,8 @@
       <c r="F64">
         <v>22</v>
       </c>
-      <c r="G64" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H64" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I64" t="s">
-        <v>2</v>
-      </c>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
@@ -2355,7 +2006,7 @@
         <v>2</v>
       </c>
       <c r="D65" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E65">
         <v>87</v>
@@ -2363,15 +2014,8 @@
       <c r="F65">
         <v>20</v>
       </c>
-      <c r="G65" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H65" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I65" t="s">
-        <v>2</v>
-      </c>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
@@ -2384,7 +2028,7 @@
         <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E66">
         <v>115</v>
@@ -2392,15 +2036,8 @@
       <c r="F66">
         <v>50</v>
       </c>
-      <c r="G66" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H66" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I66" t="s">
-        <v>2</v>
-      </c>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
@@ -2413,7 +2050,7 @@
         <v>2</v>
       </c>
       <c r="D67" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E67">
         <v>96</v>
@@ -2421,15 +2058,8 @@
       <c r="F67">
         <v>43</v>
       </c>
-      <c r="G67" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H67" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I67" t="s">
-        <v>2</v>
-      </c>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
@@ -2442,7 +2072,7 @@
         <v>2</v>
       </c>
       <c r="D68" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E68">
         <v>118</v>
@@ -2450,15 +2080,9 @@
       <c r="F68">
         <v>36</v>
       </c>
-      <c r="G68" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H68" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I68" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
@@ -2471,7 +2095,7 @@
         <v>2</v>
       </c>
       <c r="D69" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E69">
         <v>89</v>
@@ -2480,14 +2104,12 @@
         <v>21</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I69" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I69" s="4"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
@@ -2500,23 +2122,17 @@
         <v>2</v>
       </c>
       <c r="D70" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E70">
         <v>63</v>
       </c>
-      <c r="F70" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="F70" s="4"/>
       <c r="G70" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H70" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I70" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
@@ -2529,7 +2145,7 @@
         <v>1.5</v>
       </c>
       <c r="D71" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E71">
         <v>50</v>
@@ -2538,13 +2154,13 @@
         <v>6</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
@@ -2558,7 +2174,7 @@
         <v>2.5</v>
       </c>
       <c r="D72" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E72">
         <v>21</v>
@@ -2567,14 +2183,12 @@
         <v>4</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I72" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I72" s="4"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
@@ -2587,7 +2201,7 @@
         <v>2.5</v>
       </c>
       <c r="D73" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E73">
         <v>75</v>
@@ -2596,14 +2210,12 @@
         <v>14</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I73" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I73" s="4"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
@@ -2616,23 +2228,19 @@
         <v>3</v>
       </c>
       <c r="D74" t="s">
-        <v>3</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E74" s="4"/>
       <c r="F74">
         <v>12</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I74" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I74" s="4"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
@@ -2645,23 +2253,19 @@
         <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>3</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E75" s="4"/>
       <c r="F75">
         <v>12</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I75" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I75" s="4"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
@@ -2674,23 +2278,17 @@
         <v>2</v>
       </c>
       <c r="D76" t="s">
-        <v>3</v>
-      </c>
-      <c r="E76" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E76" s="4"/>
       <c r="F76">
         <v>15</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H76" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I76" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
@@ -2703,7 +2301,7 @@
         <v>2</v>
       </c>
       <c r="D77" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E77">
         <v>72</v>
@@ -2712,14 +2310,12 @@
         <v>28</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I77" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I77" s="4"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
@@ -2732,7 +2328,7 @@
         <v>4.5</v>
       </c>
       <c r="D78" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E78">
         <v>45</v>
@@ -2741,14 +2337,12 @@
         <v>15</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I78" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="I78" s="4"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
@@ -2761,7 +2355,7 @@
         <v>2.5</v>
       </c>
       <c r="D79" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E79">
         <v>58</v>
@@ -2770,14 +2364,12 @@
         <v>12</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H79" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I79" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I79" s="4"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
@@ -2790,7 +2382,7 @@
         <v>2</v>
       </c>
       <c r="D80" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E80">
         <v>27</v>
@@ -2799,14 +2391,12 @@
         <v>20</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I80" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I80" s="4"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
@@ -2819,7 +2409,7 @@
         <v>2</v>
       </c>
       <c r="D81" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E81">
         <v>13</v>
@@ -2828,13 +2418,13 @@
         <v>15</v>
       </c>
       <c r="G81" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I81" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="H81" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I81" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
@@ -2848,7 +2438,7 @@
         <v>2</v>
       </c>
       <c r="D82" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E82">
         <v>80</v>
@@ -2857,13 +2447,13 @@
         <v>16</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H82" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I82" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="I82" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
@@ -2877,23 +2467,15 @@
         <v>2.5</v>
       </c>
       <c r="D83" t="s">
-        <v>3</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E83" s="4"/>
       <c r="F83">
         <v>16</v>
       </c>
-      <c r="G83" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H83" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I83" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="G83" s="4"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="4"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
@@ -2906,7 +2488,7 @@
         <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E84">
         <v>48</v>
@@ -2915,14 +2497,12 @@
         <v>10</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I84" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I84" s="4"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
@@ -2935,7 +2515,7 @@
         <v>2</v>
       </c>
       <c r="D85" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E85">
         <v>100</v>
@@ -2944,13 +2524,13 @@
         <v>5</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
@@ -2964,7 +2544,7 @@
         <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E86">
         <v>104</v>
@@ -2973,13 +2553,13 @@
         <v>6</v>
       </c>
       <c r="G86" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
@@ -2993,7 +2573,7 @@
         <v>1.5</v>
       </c>
       <c r="D87" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E87">
         <v>57</v>
@@ -3002,14 +2582,10 @@
         <v>1</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H87" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I87" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="H87" s="4"/>
+      <c r="I87" s="4"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
@@ -3022,22 +2598,20 @@
         <v>2</v>
       </c>
       <c r="D88" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E88">
         <v>32</v>
       </c>
-      <c r="F88" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="F88" s="4"/>
       <c r="G88" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H88" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
@@ -3051,23 +2625,19 @@
         <v>2</v>
       </c>
       <c r="D89" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E89">
         <v>60</v>
       </c>
-      <c r="F89" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="F89" s="4"/>
       <c r="G89" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I89" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I89" s="4"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
@@ -3080,22 +2650,20 @@
         <v>1</v>
       </c>
       <c r="D90" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E90">
         <v>32</v>
       </c>
-      <c r="F90" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="F90" s="4"/>
       <c r="G90" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H90" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
@@ -3109,7 +2677,7 @@
         <v>2.5</v>
       </c>
       <c r="D91" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E91">
         <v>42</v>
@@ -3118,13 +2686,13 @@
         <v>4</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
@@ -3138,22 +2706,20 @@
         <v>2</v>
       </c>
       <c r="D92" t="s">
-        <v>3</v>
-      </c>
-      <c r="E92" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E92" s="4"/>
       <c r="F92">
         <v>4</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H92" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
@@ -3167,7 +2733,7 @@
         <v>1.5</v>
       </c>
       <c r="D93" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E93">
         <v>52</v>
@@ -3176,14 +2742,10 @@
         <v>3</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H93" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I93" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
@@ -3196,7 +2758,7 @@
         <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E94">
         <v>69</v>
@@ -3205,14 +2767,10 @@
         <v>5</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H94" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I94" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="H94" s="4"/>
+      <c r="I94" s="4"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
@@ -3225,7 +2783,7 @@
         <v>2</v>
       </c>
       <c r="D95" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E95">
         <v>50</v>
@@ -3234,14 +2792,10 @@
         <v>10</v>
       </c>
       <c r="G95" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H95" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I95" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H95" s="4"/>
+      <c r="I95" s="4"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
@@ -3254,7 +2808,7 @@
         <v>2</v>
       </c>
       <c r="D96" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E96">
         <v>84</v>
@@ -3263,13 +2817,13 @@
         <v>27</v>
       </c>
       <c r="G96" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H96" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I96" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
@@ -3283,7 +2837,7 @@
         <v>2</v>
       </c>
       <c r="D97" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E97">
         <v>109</v>
@@ -3292,13 +2846,13 @@
         <v>17</v>
       </c>
       <c r="G97" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H97" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I97" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
@@ -3312,7 +2866,7 @@
         <v>2</v>
       </c>
       <c r="D98" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E98">
         <v>65</v>
@@ -3321,13 +2875,13 @@
         <v>15</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H98" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I98" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
@@ -3341,7 +2895,7 @@
         <v>2</v>
       </c>
       <c r="D99" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E99">
         <v>96</v>
@@ -3350,13 +2904,11 @@
         <v>30</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H99" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="H99" s="4"/>
       <c r="I99" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
@@ -3370,7 +2922,7 @@
         <v>2</v>
       </c>
       <c r="D100" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E100">
         <v>50</v>
@@ -3379,14 +2931,10 @@
         <v>25</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H100" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I100" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="H100" s="4"/>
+      <c r="I100" s="4"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
@@ -3399,7 +2947,7 @@
         <v>2</v>
       </c>
       <c r="D101" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E101">
         <v>80</v>
@@ -3408,13 +2956,13 @@
         <v>22</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H101" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I101" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
@@ -3428,7 +2976,7 @@
         <v>2</v>
       </c>
       <c r="D102" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E102">
         <v>50</v>
@@ -3437,14 +2985,10 @@
         <v>12</v>
       </c>
       <c r="G102" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H102" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I102" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="H102" s="4"/>
+      <c r="I102" s="4"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
@@ -3457,7 +3001,7 @@
         <v>1.25</v>
       </c>
       <c r="D103" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E103">
         <v>117</v>
@@ -3466,14 +3010,10 @@
         <v>42</v>
       </c>
       <c r="G103" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H103" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I103" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="H103" s="4"/>
+      <c r="I103" s="4"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
@@ -3486,7 +3026,7 @@
         <v>2</v>
       </c>
       <c r="D104" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E104">
         <v>45</v>
@@ -3495,13 +3035,13 @@
         <v>18</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H104" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I104" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
@@ -3515,7 +3055,7 @@
         <v>1.75</v>
       </c>
       <c r="D105" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E105">
         <v>126</v>
@@ -3524,13 +3064,11 @@
         <v>30</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H105" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="H105" s="4"/>
       <c r="I105" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
@@ -3544,7 +3082,7 @@
         <v>2</v>
       </c>
       <c r="D106" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E106">
         <v>52</v>
@@ -3552,15 +3090,11 @@
       <c r="F106">
         <v>8</v>
       </c>
-      <c r="G106" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="G106" s="4"/>
       <c r="H106" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I106" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I106" s="4"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
@@ -3573,7 +3107,7 @@
         <v>2</v>
       </c>
       <c r="D107" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E107">
         <v>65</v>
@@ -3582,13 +3116,13 @@
         <v>20</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H107" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I107" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
@@ -3602,7 +3136,7 @@
         <v>2</v>
       </c>
       <c r="D108" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E108">
         <v>50</v>
@@ -3611,14 +3145,10 @@
         <v>15</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H108" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I108" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="H108" s="4"/>
+      <c r="I108" s="4"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
@@ -3631,7 +3161,7 @@
         <v>2</v>
       </c>
       <c r="D109" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E109">
         <v>104</v>
@@ -3640,14 +3170,10 @@
         <v>25</v>
       </c>
       <c r="G109" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H109" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I109" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H109" s="4"/>
+      <c r="I109" s="4"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
@@ -3660,7 +3186,7 @@
         <v>2</v>
       </c>
       <c r="D110" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E110">
         <v>35</v>
@@ -3669,13 +3195,13 @@
         <v>8</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H110" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I110" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
@@ -3689,7 +3215,7 @@
         <v>2</v>
       </c>
       <c r="D111" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E111">
         <v>73</v>
@@ -3698,13 +3224,13 @@
         <v>20</v>
       </c>
       <c r="G111" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H111" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I111" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
@@ -3718,7 +3244,7 @@
         <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E112">
         <v>110</v>
@@ -3727,14 +3253,10 @@
         <v>20</v>
       </c>
       <c r="G112" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H112" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I112" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="H112" s="4"/>
+      <c r="I112" s="4"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
@@ -3747,7 +3269,7 @@
         <v>2</v>
       </c>
       <c r="D113" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E113">
         <v>40</v>
@@ -3756,13 +3278,11 @@
         <v>8</v>
       </c>
       <c r="G113" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H113" s="4"/>
+      <c r="I113" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="H113" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I113" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
@@ -3776,23 +3296,15 @@
         <v>2</v>
       </c>
       <c r="D114" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E114">
         <v>49</v>
       </c>
-      <c r="F114" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G114" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H114" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I114" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
+      <c r="H114" s="4"/>
+      <c r="I114" s="4"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
@@ -3805,7 +3317,7 @@
         <v>1.5</v>
       </c>
       <c r="D115" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E115">
         <v>64</v>
@@ -3814,13 +3326,13 @@
         <v>4</v>
       </c>
       <c r="G115" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H115" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I115" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
@@ -3834,23 +3346,19 @@
         <v>1</v>
       </c>
       <c r="D116" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E116">
         <v>54</v>
       </c>
-      <c r="F116" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="F116" s="4"/>
       <c r="G116" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H116" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I116" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="I116" s="4"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
@@ -3863,7 +3371,7 @@
         <v>2</v>
       </c>
       <c r="D117" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E117">
         <v>100</v>
@@ -3872,13 +3380,13 @@
         <v>20</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H117" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I117" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
@@ -3892,7 +3400,7 @@
         <v>2</v>
       </c>
       <c r="D118" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E118">
         <v>36</v>
@@ -3901,13 +3409,13 @@
         <v>7</v>
       </c>
       <c r="G118" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H118" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I118" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="I118" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
@@ -3921,7 +3429,7 @@
         <v>3</v>
       </c>
       <c r="D119" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E119">
         <v>34</v>
@@ -3930,13 +3438,13 @@
         <v>2</v>
       </c>
       <c r="G119" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H119" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I119" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="I119" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
@@ -3950,7 +3458,7 @@
         <v>2</v>
       </c>
       <c r="D120" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E120">
         <v>36</v>
@@ -3959,13 +3467,13 @@
         <v>6</v>
       </c>
       <c r="G120" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H120" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I120" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="I120" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
@@ -3979,7 +3487,7 @@
         <v>2</v>
       </c>
       <c r="D121" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E121">
         <v>73</v>
@@ -3988,13 +3496,13 @@
         <v>14</v>
       </c>
       <c r="G121" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H121" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I121" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="I121" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
@@ -4008,7 +3516,7 @@
         <v>2</v>
       </c>
       <c r="D122" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E122">
         <v>111</v>
@@ -4017,13 +3525,13 @@
         <v>24</v>
       </c>
       <c r="G122" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H122" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I122" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
@@ -4037,7 +3545,7 @@
         <v>2</v>
       </c>
       <c r="D123" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E123">
         <v>91</v>
@@ -4046,13 +3554,13 @@
         <v>25</v>
       </c>
       <c r="G123" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H123" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I123" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
@@ -4066,7 +3574,7 @@
         <v>2</v>
       </c>
       <c r="D124" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E124">
         <v>135</v>
@@ -4075,13 +3583,13 @@
         <v>41</v>
       </c>
       <c r="G124" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H124" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I124" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
@@ -4095,7 +3603,7 @@
         <v>2</v>
       </c>
       <c r="D125" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E125">
         <v>47</v>
@@ -4104,13 +3612,13 @@
         <v>13</v>
       </c>
       <c r="G125" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H125" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I125" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
@@ -4124,7 +3632,7 @@
         <v>2</v>
       </c>
       <c r="D126" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E126">
         <v>78</v>
@@ -4133,13 +3641,13 @@
         <v>38</v>
       </c>
       <c r="G126" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H126" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I126" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
@@ -4153,7 +3661,7 @@
         <v>2</v>
       </c>
       <c r="D127" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E127">
         <v>65</v>
@@ -4162,13 +3670,13 @@
         <v>14</v>
       </c>
       <c r="G127" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H127" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I127" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
@@ -4182,7 +3690,7 @@
         <v>2</v>
       </c>
       <c r="D128" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E128">
         <v>55</v>
@@ -4191,13 +3699,13 @@
         <v>21</v>
       </c>
       <c r="G128" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H128" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I128" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="I128" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
@@ -4211,7 +3719,7 @@
         <v>2.5</v>
       </c>
       <c r="D129" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E129">
         <v>59</v>
@@ -4220,13 +3728,13 @@
         <v>17</v>
       </c>
       <c r="G129" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H129" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I129" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="I129" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
@@ -4240,7 +3748,7 @@
         <v>2</v>
       </c>
       <c r="D130" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E130">
         <v>61</v>
@@ -4249,13 +3757,13 @@
         <v>15</v>
       </c>
       <c r="G130" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H130" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I130" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
@@ -4269,7 +3777,7 @@
         <v>0.75</v>
       </c>
       <c r="D131" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E131">
         <v>68</v>
@@ -4278,13 +3786,13 @@
         <v>16</v>
       </c>
       <c r="G131" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H131" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I131" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
@@ -4298,7 +3806,7 @@
         <v>2</v>
       </c>
       <c r="D132" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E132">
         <v>43</v>
@@ -4307,13 +3815,13 @@
         <v>11</v>
       </c>
       <c r="G132" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H132" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I132" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="I132" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.2">
@@ -4327,7 +3835,7 @@
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E133">
         <v>74</v>
@@ -4336,13 +3844,13 @@
         <v>20</v>
       </c>
       <c r="G133" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H133" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I133" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
@@ -4356,7 +3864,7 @@
         <v>2</v>
       </c>
       <c r="D134" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E134">
         <v>80</v>
@@ -4365,14 +3873,12 @@
         <v>15</v>
       </c>
       <c r="G134" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H134" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I134" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="I134" s="4"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
@@ -4385,7 +3891,7 @@
         <v>2</v>
       </c>
       <c r="D135" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E135">
         <v>76</v>
@@ -4394,13 +3900,13 @@
         <v>13</v>
       </c>
       <c r="G135" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H135" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I135" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
@@ -4414,7 +3920,7 @@
         <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E136">
         <v>70</v>
@@ -4423,13 +3929,13 @@
         <v>20</v>
       </c>
       <c r="G136" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H136" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I136" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
@@ -4443,22 +3949,20 @@
         <v>2</v>
       </c>
       <c r="D137" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E137">
         <v>80</v>
       </c>
-      <c r="F137" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="F137" s="4"/>
       <c r="G137" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H137" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I137" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="I137" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -4481,18 +3985,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>